<commit_message>
So I need a event handler, which isn't a problem I just wanted to make sure.
</commit_message>
<xml_diff>
--- a/Ontwerp document.xlsx
+++ b/Ontwerp document.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7628E9D-B0C0-4E1D-919B-E50069C48538}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>Action</t>
   </si>
@@ -145,14 +146,31 @@
   </si>
   <si>
     <t>Get light hours a day for new plant</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Go back to user menu</t>
+  </si>
+  <si>
+    <t>remove this, it's gonna suck</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -168,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -241,32 +259,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -543,21 +582,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -566,227 +607,242 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7" t="s">
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8" t="s">
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8" t="s">
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D18" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -796,5 +852,6 @@
     <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Small changes for merge
</commit_message>
<xml_diff>
--- a/Ontwerp document.xlsx
+++ b/Ontwerp document.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Action</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Get light hours a day for new plant</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Go back to user menu</t>
   </si>
 </sst>
 </file>
@@ -251,9 +257,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -262,6 +265,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -544,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,222 +577,232 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="D11" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="D12" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="D13" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7" t="s">
+      <c r="D14" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8" t="s">
+      <c r="D16" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8" t="s">
+      <c r="D17" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>